<commit_message>
chatgpt is doing weird shit
</commit_message>
<xml_diff>
--- a/data/Leetcode_question_bank_V01.xlsx
+++ b/data/Leetcode_question_bank_V01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fhans/Documents/GenerativeBenchmarking/clone-anonymous-github/ChatGPT-Study-2757/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EC93D5-C436-E34E-9607-DAB0443D8DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59B3C24-F033-6E44-9996-53D81CA0394E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -9472,11 +9472,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4045"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="I111" sqref="I111"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -102514,6 +102518,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G4045" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>